<commit_message>
seperated R50 and R25
</commit_message>
<xml_diff>
--- a/Results/0 Compiled Results for Manuscript.xlsx
+++ b/Results/0 Compiled Results for Manuscript.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tigermailauburn-my.sharepoint.com/personal/bzm0094_auburn_edu/Documents/Collaboration/Ngbede M/Agrivoltaics-alabama/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1725" documentId="11_F25DC773A252ABDACC1048E1719A46A65ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C5AD9EB-218E-43C4-8DED-D33915F6BC2E}"/>
+  <xr:revisionPtr revIDLastSave="1726" documentId="11_F25DC773A252ABDACC1048E1719A46A65ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AC3A9A2-074C-4001-8B47-D880571ACBC7}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TAV" sheetId="1" r:id="rId1"/>
@@ -980,11 +980,17 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -992,8 +998,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1013,9 +1031,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1025,26 +1040,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -8540,10 +8540,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -9603,7 +9599,7 @@
       <c r="D1" s="67"/>
       <c r="E1" s="67"/>
       <c r="F1" s="67"/>
-      <c r="G1" s="70" t="s">
+      <c r="G1" s="68" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="67"/>
@@ -9730,62 +9726,62 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="X2" s="41"/>
-      <c r="Y2" s="68" t="s">
+      <c r="Y2" s="70" t="s">
         <v>94</v>
       </c>
-      <c r="Z2" s="69"/>
-      <c r="AA2" s="69"/>
-      <c r="AB2" s="69"/>
-      <c r="AC2" s="66" t="s">
+      <c r="Z2" s="71"/>
+      <c r="AA2" s="71"/>
+      <c r="AB2" s="71"/>
+      <c r="AC2" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="AD2" s="66"/>
-      <c r="AE2" s="66"/>
-      <c r="AF2" s="66" t="s">
+      <c r="AD2" s="69"/>
+      <c r="AE2" s="69"/>
+      <c r="AF2" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="AG2" s="66"/>
-      <c r="AH2" s="66"/>
-      <c r="AI2" s="66" t="s">
+      <c r="AG2" s="69"/>
+      <c r="AH2" s="69"/>
+      <c r="AI2" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="AJ2" s="66"/>
-      <c r="AK2" s="66"/>
-      <c r="AL2" s="66" t="s">
+      <c r="AJ2" s="69"/>
+      <c r="AK2" s="69"/>
+      <c r="AL2" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="AM2" s="66"/>
-      <c r="AN2" s="66"/>
-      <c r="AO2" s="66" t="s">
+      <c r="AM2" s="69"/>
+      <c r="AN2" s="69"/>
+      <c r="AO2" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="AP2" s="66"/>
-      <c r="AQ2" s="66"/>
-      <c r="AR2" s="66" t="s">
+      <c r="AP2" s="69"/>
+      <c r="AQ2" s="69"/>
+      <c r="AR2" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="AS2" s="66"/>
-      <c r="AT2" s="66"/>
-      <c r="AU2" s="66" t="s">
+      <c r="AS2" s="69"/>
+      <c r="AT2" s="69"/>
+      <c r="AU2" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="AV2" s="66"/>
-      <c r="AW2" s="66"/>
-      <c r="AX2" s="66" t="s">
+      <c r="AV2" s="69"/>
+      <c r="AW2" s="69"/>
+      <c r="AX2" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="AY2" s="66"/>
-      <c r="AZ2" s="66"/>
-      <c r="BA2" s="66" t="s">
+      <c r="AY2" s="69"/>
+      <c r="AZ2" s="69"/>
+      <c r="BA2" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="BB2" s="66"/>
-      <c r="BC2" s="66"/>
-      <c r="BD2" s="66" t="s">
+      <c r="BB2" s="69"/>
+      <c r="BC2" s="69"/>
+      <c r="BD2" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="BE2" s="66"/>
-      <c r="BF2" s="66"/>
+      <c r="BE2" s="69"/>
+      <c r="BF2" s="69"/>
     </row>
     <row r="3" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -9806,7 +9802,7 @@
       <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="70" t="s">
+      <c r="G3" s="68" t="s">
         <v>91</v>
       </c>
       <c r="H3" s="67"/>
@@ -12235,22 +12231,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G3:U3"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="Y3:AB3"/>
-    <mergeCell ref="AC1:AH1"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AL2:AN2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="Y2:AB2"/>
-    <mergeCell ref="Y1:AB1"/>
     <mergeCell ref="BD2:BF2"/>
     <mergeCell ref="BA1:BF1"/>
     <mergeCell ref="AU1:AZ1"/>
@@ -12261,6 +12241,22 @@
     <mergeCell ref="AO2:AQ2"/>
     <mergeCell ref="AU2:AW2"/>
     <mergeCell ref="BA2:BC2"/>
+    <mergeCell ref="Y3:AB3"/>
+    <mergeCell ref="AC1:AH1"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="Y2:AB2"/>
+    <mergeCell ref="Y1:AB1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G3:U3"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="57" orientation="landscape" r:id="rId1"/>
@@ -12306,7 +12302,7 @@
       <c r="D1" s="67"/>
       <c r="E1" s="67"/>
       <c r="F1" s="67"/>
-      <c r="G1" s="70" t="s">
+      <c r="G1" s="68" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="67"/>
@@ -12433,62 +12429,62 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="W2" s="41"/>
-      <c r="X2" s="66" t="s">
+      <c r="X2" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="66"/>
-      <c r="Z2" s="66"/>
-      <c r="AA2" s="66"/>
-      <c r="AB2" s="66" t="s">
+      <c r="Y2" s="69"/>
+      <c r="Z2" s="69"/>
+      <c r="AA2" s="69"/>
+      <c r="AB2" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="AC2" s="66"/>
-      <c r="AD2" s="66"/>
-      <c r="AE2" s="66" t="s">
+      <c r="AC2" s="69"/>
+      <c r="AD2" s="69"/>
+      <c r="AE2" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="AF2" s="66"/>
-      <c r="AG2" s="66"/>
-      <c r="AH2" s="66" t="s">
+      <c r="AF2" s="69"/>
+      <c r="AG2" s="69"/>
+      <c r="AH2" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="AI2" s="66"/>
-      <c r="AJ2" s="66"/>
-      <c r="AK2" s="66" t="s">
+      <c r="AI2" s="69"/>
+      <c r="AJ2" s="69"/>
+      <c r="AK2" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="AL2" s="66"/>
-      <c r="AM2" s="66"/>
-      <c r="AN2" s="66" t="s">
+      <c r="AL2" s="69"/>
+      <c r="AM2" s="69"/>
+      <c r="AN2" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="AO2" s="66"/>
-      <c r="AP2" s="66"/>
-      <c r="AQ2" s="66" t="s">
+      <c r="AO2" s="69"/>
+      <c r="AP2" s="69"/>
+      <c r="AQ2" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="AR2" s="66"/>
-      <c r="AS2" s="66"/>
-      <c r="AT2" s="66" t="s">
+      <c r="AR2" s="69"/>
+      <c r="AS2" s="69"/>
+      <c r="AT2" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="AU2" s="66"/>
-      <c r="AV2" s="66"/>
-      <c r="AW2" s="66" t="s">
+      <c r="AU2" s="69"/>
+      <c r="AV2" s="69"/>
+      <c r="AW2" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="AX2" s="66"/>
-      <c r="AY2" s="66"/>
-      <c r="AZ2" s="66" t="s">
+      <c r="AX2" s="69"/>
+      <c r="AY2" s="69"/>
+      <c r="AZ2" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="BA2" s="66"/>
-      <c r="BB2" s="66"/>
-      <c r="BC2" s="66" t="s">
+      <c r="BA2" s="69"/>
+      <c r="BB2" s="69"/>
+      <c r="BC2" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="BD2" s="66"/>
-      <c r="BE2" s="66"/>
+      <c r="BD2" s="69"/>
+      <c r="BE2" s="69"/>
     </row>
     <row r="3" spans="1:57" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -12509,7 +12505,7 @@
       <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="70" t="s">
+      <c r="G3" s="68" t="s">
         <v>92</v>
       </c>
       <c r="H3" s="67"/>
@@ -12703,36 +12699,36 @@
       <c r="AA4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="AB4" s="87"/>
-      <c r="AC4" s="87"/>
-      <c r="AD4" s="87"/>
-      <c r="AE4" s="87"/>
-      <c r="AF4" s="87"/>
-      <c r="AG4" s="87"/>
-      <c r="AH4" s="87"/>
-      <c r="AI4" s="87"/>
-      <c r="AJ4" s="87"/>
-      <c r="AK4" s="87"/>
-      <c r="AL4" s="87"/>
-      <c r="AM4" s="87"/>
-      <c r="AN4" s="87"/>
-      <c r="AO4" s="87"/>
-      <c r="AP4" s="87"/>
-      <c r="AQ4" s="87"/>
-      <c r="AR4" s="87"/>
-      <c r="AS4" s="87"/>
-      <c r="AT4" s="87"/>
-      <c r="AU4" s="87"/>
-      <c r="AV4" s="87"/>
-      <c r="AW4" s="87"/>
-      <c r="AX4" s="87"/>
-      <c r="AY4" s="87"/>
-      <c r="AZ4" s="87"/>
-      <c r="BA4" s="87"/>
-      <c r="BB4" s="87"/>
-      <c r="BC4" s="87"/>
-      <c r="BD4" s="87"/>
-      <c r="BE4" s="87"/>
+      <c r="AB4" s="66"/>
+      <c r="AC4" s="66"/>
+      <c r="AD4" s="66"/>
+      <c r="AE4" s="66"/>
+      <c r="AF4" s="66"/>
+      <c r="AG4" s="66"/>
+      <c r="AH4" s="66"/>
+      <c r="AI4" s="66"/>
+      <c r="AJ4" s="66"/>
+      <c r="AK4" s="66"/>
+      <c r="AL4" s="66"/>
+      <c r="AM4" s="66"/>
+      <c r="AN4" s="66"/>
+      <c r="AO4" s="66"/>
+      <c r="AP4" s="66"/>
+      <c r="AQ4" s="66"/>
+      <c r="AR4" s="66"/>
+      <c r="AS4" s="66"/>
+      <c r="AT4" s="66"/>
+      <c r="AU4" s="66"/>
+      <c r="AV4" s="66"/>
+      <c r="AW4" s="66"/>
+      <c r="AX4" s="66"/>
+      <c r="AY4" s="66"/>
+      <c r="AZ4" s="66"/>
+      <c r="BA4" s="66"/>
+      <c r="BB4" s="66"/>
+      <c r="BC4" s="66"/>
+      <c r="BD4" s="66"/>
+      <c r="BE4" s="66"/>
     </row>
     <row r="5" spans="1:57" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -12814,123 +12810,123 @@
         <v>0.04</v>
       </c>
       <c r="AB5" s="44">
-        <f>G12-G4</f>
+        <f t="shared" ref="AB5:AD8" si="0">G12-G4</f>
         <v>0</v>
       </c>
       <c r="AC5" s="44">
-        <f>H12-H4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD5" s="44">
-        <f>I12-I4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AE5" s="44">
-        <f>G16-G8</f>
+        <f t="shared" ref="AE5:AG8" si="1">G16-G8</f>
         <v>0</v>
       </c>
       <c r="AF5" s="44">
-        <f>H16-H8</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AG5" s="44">
-        <f>I16-I8</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AH5" s="44">
-        <f>J12-J4</f>
+        <f t="shared" ref="AH5:AJ8" si="2">J12-J4</f>
         <v>-3296</v>
       </c>
       <c r="AI5" s="44">
-        <f>K12-K4</f>
+        <f t="shared" si="2"/>
         <v>-3827</v>
       </c>
       <c r="AJ5" s="44">
-        <f>L12-L4</f>
+        <f t="shared" si="2"/>
         <v>-4820</v>
       </c>
       <c r="AK5" s="44">
-        <f>J16-J8</f>
+        <f t="shared" ref="AK5:AM8" si="3">J16-J8</f>
         <v>-3586</v>
       </c>
       <c r="AL5" s="44">
-        <f>K16-K8</f>
+        <f t="shared" si="3"/>
         <v>-3975</v>
       </c>
       <c r="AM5" s="44">
-        <f>L16-L8</f>
+        <f t="shared" si="3"/>
         <v>-4365</v>
       </c>
       <c r="AN5" s="44">
-        <f>M12-M4</f>
+        <f t="shared" ref="AN5:AP8" si="4">M12-M4</f>
         <v>-7691</v>
       </c>
       <c r="AO5" s="44">
-        <f>N12-N4</f>
+        <f t="shared" si="4"/>
         <v>-8929</v>
       </c>
       <c r="AP5" s="44">
-        <f>O12-O4</f>
+        <f t="shared" si="4"/>
         <v>-11247</v>
       </c>
       <c r="AQ5" s="44">
-        <f>M16-M8</f>
+        <f t="shared" ref="AQ5:AS8" si="5">M16-M8</f>
         <v>-8367</v>
       </c>
       <c r="AR5" s="44">
-        <f>N16-N8</f>
+        <f t="shared" si="5"/>
         <v>-9275</v>
       </c>
       <c r="AS5" s="44">
-        <f>O16-O8</f>
+        <f t="shared" si="5"/>
         <v>-10185</v>
       </c>
       <c r="AT5" s="44">
-        <f>P12-P4</f>
+        <f t="shared" ref="AT5:AV8" si="6">P12-P4</f>
         <v>-12086</v>
       </c>
       <c r="AU5" s="44">
-        <f>Q12-Q4</f>
+        <f t="shared" si="6"/>
         <v>-14033</v>
       </c>
       <c r="AV5" s="44">
-        <f>R12-R4</f>
+        <f t="shared" si="6"/>
         <v>-17674</v>
       </c>
       <c r="AW5" s="44">
-        <f>P16-P8</f>
+        <f t="shared" ref="AW5:AY8" si="7">P16-P8</f>
         <v>-13148</v>
       </c>
       <c r="AX5" s="44">
-        <f>Q16-Q8</f>
+        <f t="shared" si="7"/>
         <v>-14576</v>
       </c>
       <c r="AY5" s="44">
-        <f>R16-R8</f>
+        <f t="shared" si="7"/>
         <v>-16005</v>
       </c>
       <c r="AZ5" s="44">
-        <f>S12-S4</f>
+        <f t="shared" ref="AZ5:BB8" si="8">S12-S4</f>
         <v>-16480</v>
       </c>
       <c r="BA5" s="44">
-        <f>T12-T4</f>
+        <f t="shared" si="8"/>
         <v>-19135</v>
       </c>
       <c r="BB5" s="44">
-        <f>U12-U4</f>
+        <f t="shared" si="8"/>
         <v>-24100</v>
       </c>
       <c r="BC5" s="44">
-        <f>S16-S8</f>
+        <f t="shared" ref="BC5:BE8" si="9">S16-S8</f>
         <v>-17928</v>
       </c>
       <c r="BD5" s="44">
-        <f>T16-T8</f>
+        <f t="shared" si="9"/>
         <v>-19876</v>
       </c>
       <c r="BE5" s="44">
-        <f>U16-U8</f>
+        <f t="shared" si="9"/>
         <v>-21825</v>
       </c>
     </row>
@@ -13014,123 +13010,123 @@
         <v>0.04</v>
       </c>
       <c r="AB6" s="44">
-        <f>G13-G5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AC6" s="44">
-        <f>H13-H5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD6" s="44">
-        <f>I13-I5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AE6" s="44">
-        <f>G17-G9</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF6" s="44">
-        <f>H17-H9</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AG6" s="44">
-        <f>I17-I9</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AH6" s="44">
-        <f>J13-J5</f>
+        <f t="shared" si="2"/>
         <v>-3296</v>
       </c>
       <c r="AI6" s="44">
-        <f>K13-K5</f>
+        <f t="shared" si="2"/>
         <v>-3827</v>
       </c>
       <c r="AJ6" s="44">
-        <f>L13-L5</f>
+        <f t="shared" si="2"/>
         <v>-4820</v>
       </c>
       <c r="AK6" s="44">
-        <f>J17-J9</f>
+        <f t="shared" si="3"/>
         <v>-3586</v>
       </c>
       <c r="AL6" s="44">
-        <f>K17-K9</f>
+        <f t="shared" si="3"/>
         <v>-3975</v>
       </c>
       <c r="AM6" s="44">
-        <f>L17-L9</f>
+        <f t="shared" si="3"/>
         <v>-4365</v>
       </c>
       <c r="AN6" s="44">
-        <f>M13-M5</f>
+        <f t="shared" si="4"/>
         <v>-7691</v>
       </c>
       <c r="AO6" s="44">
-        <f>N13-N5</f>
+        <f t="shared" si="4"/>
         <v>-8930</v>
       </c>
       <c r="AP6" s="44">
-        <f>O13-O5</f>
+        <f t="shared" si="4"/>
         <v>-11247</v>
       </c>
       <c r="AQ6" s="44">
-        <f>M17-M9</f>
+        <f t="shared" si="5"/>
         <v>-8366</v>
       </c>
       <c r="AR6" s="44">
-        <f>N17-N9</f>
+        <f t="shared" si="5"/>
         <v>-9276</v>
       </c>
       <c r="AS6" s="44">
-        <f>O17-O9</f>
+        <f t="shared" si="5"/>
         <v>-10185</v>
       </c>
       <c r="AT6" s="44">
-        <f>P13-P5</f>
+        <f t="shared" si="6"/>
         <v>-12086</v>
       </c>
       <c r="AU6" s="44">
-        <f>Q13-Q5</f>
+        <f t="shared" si="6"/>
         <v>-14033</v>
       </c>
       <c r="AV6" s="44">
-        <f>R13-R5</f>
+        <f t="shared" si="6"/>
         <v>-17674</v>
       </c>
       <c r="AW6" s="44">
-        <f>P17-P9</f>
+        <f t="shared" si="7"/>
         <v>-13148</v>
       </c>
       <c r="AX6" s="44">
-        <f>Q17-Q9</f>
+        <f t="shared" si="7"/>
         <v>-14577</v>
       </c>
       <c r="AY6" s="44">
-        <f>R17-R9</f>
+        <f t="shared" si="7"/>
         <v>-16004</v>
       </c>
       <c r="AZ6" s="44">
-        <f>S13-S5</f>
+        <f t="shared" si="8"/>
         <v>-16481</v>
       </c>
       <c r="BA6" s="44">
-        <f>T13-T5</f>
+        <f t="shared" si="8"/>
         <v>-19136</v>
       </c>
       <c r="BB6" s="44">
-        <f>U13-U5</f>
+        <f t="shared" si="8"/>
         <v>-24101</v>
       </c>
       <c r="BC6" s="44">
-        <f>S17-S9</f>
+        <f t="shared" si="9"/>
         <v>-17929</v>
       </c>
       <c r="BD6" s="44">
-        <f>T17-T9</f>
+        <f t="shared" si="9"/>
         <v>-19877</v>
       </c>
       <c r="BE6" s="44">
-        <f>U17-U9</f>
+        <f t="shared" si="9"/>
         <v>-21825</v>
       </c>
     </row>
@@ -13214,123 +13210,123 @@
         <v>0.04</v>
       </c>
       <c r="AB7" s="44">
-        <f>G14-G6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AC7" s="44">
-        <f>H14-H6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD7" s="44">
-        <f>I14-I6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AE7" s="44">
-        <f>G18-G10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF7" s="44">
-        <f>H18-H10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AG7" s="44">
-        <f>I18-I10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AH7" s="44">
-        <f>J14-J6</f>
+        <f t="shared" si="2"/>
         <v>-3296</v>
       </c>
       <c r="AI7" s="44">
-        <f>K14-K6</f>
+        <f t="shared" si="2"/>
         <v>-3827</v>
       </c>
       <c r="AJ7" s="44">
-        <f>L14-L6</f>
+        <f t="shared" si="2"/>
         <v>-4820</v>
       </c>
       <c r="AK7" s="44">
-        <f>J18-J10</f>
+        <f t="shared" si="3"/>
         <v>-3586</v>
       </c>
       <c r="AL7" s="44">
-        <f>K18-K10</f>
+        <f t="shared" si="3"/>
         <v>-3976</v>
       </c>
       <c r="AM7" s="44">
-        <f>L18-L10</f>
+        <f t="shared" si="3"/>
         <v>-4365</v>
       </c>
       <c r="AN7" s="44">
-        <f>M14-M6</f>
+        <f t="shared" si="4"/>
         <v>-7691</v>
       </c>
       <c r="AO7" s="44">
-        <f>N14-N6</f>
+        <f t="shared" si="4"/>
         <v>-8930</v>
       </c>
       <c r="AP7" s="44">
-        <f>O14-O6</f>
+        <f t="shared" si="4"/>
         <v>-11247</v>
       </c>
       <c r="AQ7" s="44">
-        <f>M18-M10</f>
+        <f t="shared" si="5"/>
         <v>-8367</v>
       </c>
       <c r="AR7" s="44">
-        <f>N18-N10</f>
+        <f t="shared" si="5"/>
         <v>-9276</v>
       </c>
       <c r="AS7" s="44">
-        <f>O18-O10</f>
+        <f t="shared" si="5"/>
         <v>-10185</v>
       </c>
       <c r="AT7" s="44">
-        <f>P14-P6</f>
+        <f t="shared" si="6"/>
         <v>-12086</v>
       </c>
       <c r="AU7" s="44">
-        <f>Q14-Q6</f>
+        <f t="shared" si="6"/>
         <v>-14033</v>
       </c>
       <c r="AV7" s="44">
-        <f>R14-R6</f>
+        <f t="shared" si="6"/>
         <v>-17674</v>
       </c>
       <c r="AW7" s="44">
-        <f>P18-P10</f>
+        <f t="shared" si="7"/>
         <v>-13148</v>
       </c>
       <c r="AX7" s="44">
-        <f>Q18-Q10</f>
+        <f t="shared" si="7"/>
         <v>-14577</v>
       </c>
       <c r="AY7" s="44">
-        <f>R18-R10</f>
+        <f t="shared" si="7"/>
         <v>-16005</v>
       </c>
       <c r="AZ7" s="44">
-        <f>S14-S6</f>
+        <f t="shared" si="8"/>
         <v>-16481</v>
       </c>
       <c r="BA7" s="44">
-        <f>T14-T6</f>
+        <f t="shared" si="8"/>
         <v>-19135</v>
       </c>
       <c r="BB7" s="44">
-        <f>U14-U6</f>
+        <f t="shared" si="8"/>
         <v>-24100</v>
       </c>
       <c r="BC7" s="44">
-        <f>S18-S10</f>
+        <f t="shared" si="9"/>
         <v>-17929</v>
       </c>
       <c r="BD7" s="44">
-        <f>T18-T10</f>
+        <f t="shared" si="9"/>
         <v>-19876</v>
       </c>
       <c r="BE7" s="44">
-        <f>U18-U10</f>
+        <f t="shared" si="9"/>
         <v>-21825</v>
       </c>
     </row>
@@ -13414,123 +13410,123 @@
         <v>0.04</v>
       </c>
       <c r="AB8" s="44">
-        <f>G15-G7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AC8" s="44">
-        <f>H15-H7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD8" s="44">
-        <f>I15-I7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AE8" s="44">
-        <f>G19-G11</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF8" s="44">
-        <f>H19-H11</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AG8" s="44">
-        <f>I19-I11</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AH8" s="44">
-        <f>J15-J7</f>
+        <f t="shared" si="2"/>
         <v>-3296</v>
       </c>
       <c r="AI8" s="44">
-        <f>K15-K7</f>
+        <f t="shared" si="2"/>
         <v>-3827</v>
       </c>
       <c r="AJ8" s="44">
-        <f>L15-L7</f>
+        <f t="shared" si="2"/>
         <v>-4820</v>
       </c>
       <c r="AK8" s="44">
-        <f>J19-J11</f>
+        <f t="shared" si="3"/>
         <v>-3585</v>
       </c>
       <c r="AL8" s="44">
-        <f>K19-K11</f>
+        <f t="shared" si="3"/>
         <v>-3975</v>
       </c>
       <c r="AM8" s="44">
-        <f>L19-L11</f>
+        <f t="shared" si="3"/>
         <v>-4365</v>
       </c>
       <c r="AN8" s="44">
-        <f>M15-M7</f>
+        <f t="shared" si="4"/>
         <v>-7691</v>
       </c>
       <c r="AO8" s="44">
-        <f>N15-N7</f>
+        <f t="shared" si="4"/>
         <v>-8930</v>
       </c>
       <c r="AP8" s="44">
-        <f>O15-O7</f>
+        <f t="shared" si="4"/>
         <v>-11247</v>
       </c>
       <c r="AQ8" s="44">
-        <f>M19-M11</f>
+        <f t="shared" si="5"/>
         <v>-8366</v>
       </c>
       <c r="AR8" s="44">
-        <f>N19-N11</f>
+        <f t="shared" si="5"/>
         <v>-9276</v>
       </c>
       <c r="AS8" s="44">
-        <f>O19-O11</f>
+        <f t="shared" si="5"/>
         <v>-10184</v>
       </c>
       <c r="AT8" s="44">
-        <f>P15-P7</f>
+        <f t="shared" si="6"/>
         <v>-12086</v>
       </c>
       <c r="AU8" s="44">
-        <f>Q15-Q7</f>
+        <f t="shared" si="6"/>
         <v>-14033</v>
       </c>
       <c r="AV8" s="44">
-        <f>R15-R7</f>
+        <f t="shared" si="6"/>
         <v>-17673</v>
       </c>
       <c r="AW8" s="44">
-        <f>P19-P11</f>
+        <f t="shared" si="7"/>
         <v>-13148</v>
       </c>
       <c r="AX8" s="44">
-        <f>Q19-Q11</f>
+        <f t="shared" si="7"/>
         <v>-14577</v>
       </c>
       <c r="AY8" s="44">
-        <f>R19-R11</f>
+        <f t="shared" si="7"/>
         <v>-16005</v>
       </c>
       <c r="AZ8" s="44">
-        <f>S15-S7</f>
+        <f t="shared" si="8"/>
         <v>-16481</v>
       </c>
       <c r="BA8" s="44">
-        <f>T15-T7</f>
+        <f t="shared" si="8"/>
         <v>-19136</v>
       </c>
       <c r="BB8" s="44">
-        <f>U15-U7</f>
+        <f t="shared" si="8"/>
         <v>-24101</v>
       </c>
       <c r="BC8" s="44">
-        <f>S19-S11</f>
+        <f t="shared" si="9"/>
         <v>-17928</v>
       </c>
       <c r="BD8" s="44">
-        <f>T19-T11</f>
+        <f t="shared" si="9"/>
         <v>-19877</v>
       </c>
       <c r="BE8" s="44">
-        <f>U19-U11</f>
+        <f t="shared" si="9"/>
         <v>-21825</v>
       </c>
     </row>
@@ -14266,63 +14262,63 @@
         <v>0.04</v>
       </c>
       <c r="G20" s="33">
-        <f>G12-G4</f>
+        <f t="shared" ref="G20:U20" si="10">G12-G4</f>
         <v>0</v>
       </c>
       <c r="H20" s="33">
-        <f>H12-H4</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I20" s="33">
-        <f>I12-I4</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J20" s="33">
-        <f>J12-J4</f>
+        <f t="shared" si="10"/>
         <v>-3296</v>
       </c>
       <c r="K20" s="33">
-        <f>K12-K4</f>
+        <f t="shared" si="10"/>
         <v>-3827</v>
       </c>
       <c r="L20" s="33">
-        <f>L12-L4</f>
+        <f t="shared" si="10"/>
         <v>-4820</v>
       </c>
       <c r="M20" s="33">
-        <f>M12-M4</f>
+        <f t="shared" si="10"/>
         <v>-7691</v>
       </c>
       <c r="N20" s="33">
-        <f>N12-N4</f>
+        <f t="shared" si="10"/>
         <v>-8929</v>
       </c>
       <c r="O20" s="33">
-        <f>O12-O4</f>
+        <f t="shared" si="10"/>
         <v>-11247</v>
       </c>
       <c r="P20" s="33">
-        <f>P12-P4</f>
+        <f t="shared" si="10"/>
         <v>-12086</v>
       </c>
       <c r="Q20" s="33">
-        <f>Q12-Q4</f>
+        <f t="shared" si="10"/>
         <v>-14033</v>
       </c>
       <c r="R20" s="33">
-        <f>R12-R4</f>
+        <f t="shared" si="10"/>
         <v>-17674</v>
       </c>
       <c r="S20" s="33">
-        <f>S12-S4</f>
+        <f t="shared" si="10"/>
         <v>-16480</v>
       </c>
       <c r="T20" s="33">
-        <f>T12-T4</f>
+        <f t="shared" si="10"/>
         <v>-19135</v>
       </c>
       <c r="U20" s="33">
-        <f>U12-U4</f>
+        <f t="shared" si="10"/>
         <v>-24100</v>
       </c>
     </row>
@@ -14343,63 +14339,63 @@
         <v>0.04</v>
       </c>
       <c r="G21" s="33">
-        <f>G13-G5</f>
+        <f t="shared" ref="G21:U21" si="11">G13-G5</f>
         <v>0</v>
       </c>
       <c r="H21" s="33">
-        <f>H13-H5</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="I21" s="33">
-        <f>I13-I5</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="J21" s="33">
-        <f>J13-J5</f>
+        <f t="shared" si="11"/>
         <v>-3296</v>
       </c>
       <c r="K21" s="33">
-        <f>K13-K5</f>
+        <f t="shared" si="11"/>
         <v>-3827</v>
       </c>
       <c r="L21" s="33">
-        <f>L13-L5</f>
+        <f t="shared" si="11"/>
         <v>-4820</v>
       </c>
       <c r="M21" s="33">
-        <f>M13-M5</f>
+        <f t="shared" si="11"/>
         <v>-7691</v>
       </c>
       <c r="N21" s="33">
-        <f>N13-N5</f>
+        <f t="shared" si="11"/>
         <v>-8930</v>
       </c>
       <c r="O21" s="33">
-        <f>O13-O5</f>
+        <f t="shared" si="11"/>
         <v>-11247</v>
       </c>
       <c r="P21" s="33">
-        <f>P13-P5</f>
+        <f t="shared" si="11"/>
         <v>-12086</v>
       </c>
       <c r="Q21" s="33">
-        <f>Q13-Q5</f>
+        <f t="shared" si="11"/>
         <v>-14033</v>
       </c>
       <c r="R21" s="33">
-        <f>R13-R5</f>
+        <f t="shared" si="11"/>
         <v>-17674</v>
       </c>
       <c r="S21" s="33">
-        <f>S13-S5</f>
+        <f t="shared" si="11"/>
         <v>-16481</v>
       </c>
       <c r="T21" s="33">
-        <f>T13-T5</f>
+        <f t="shared" si="11"/>
         <v>-19136</v>
       </c>
       <c r="U21" s="33">
-        <f>U13-U5</f>
+        <f t="shared" si="11"/>
         <v>-24101</v>
       </c>
     </row>
@@ -14420,63 +14416,63 @@
         <v>0.04</v>
       </c>
       <c r="G22" s="33">
-        <f>G14-G6</f>
+        <f t="shared" ref="G22:U22" si="12">G14-G6</f>
         <v>0</v>
       </c>
       <c r="H22" s="33">
-        <f>H14-H6</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I22" s="33">
-        <f>I14-I6</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="J22" s="33">
-        <f>J14-J6</f>
+        <f t="shared" si="12"/>
         <v>-3296</v>
       </c>
       <c r="K22" s="33">
-        <f>K14-K6</f>
+        <f t="shared" si="12"/>
         <v>-3827</v>
       </c>
       <c r="L22" s="33">
-        <f>L14-L6</f>
+        <f t="shared" si="12"/>
         <v>-4820</v>
       </c>
       <c r="M22" s="33">
-        <f>M14-M6</f>
+        <f t="shared" si="12"/>
         <v>-7691</v>
       </c>
       <c r="N22" s="33">
-        <f>N14-N6</f>
+        <f t="shared" si="12"/>
         <v>-8930</v>
       </c>
       <c r="O22" s="33">
-        <f>O14-O6</f>
+        <f t="shared" si="12"/>
         <v>-11247</v>
       </c>
       <c r="P22" s="33">
-        <f>P14-P6</f>
+        <f t="shared" si="12"/>
         <v>-12086</v>
       </c>
       <c r="Q22" s="33">
-        <f>Q14-Q6</f>
+        <f t="shared" si="12"/>
         <v>-14033</v>
       </c>
       <c r="R22" s="33">
-        <f>R14-R6</f>
+        <f t="shared" si="12"/>
         <v>-17674</v>
       </c>
       <c r="S22" s="33">
-        <f>S14-S6</f>
+        <f t="shared" si="12"/>
         <v>-16481</v>
       </c>
       <c r="T22" s="33">
-        <f>T14-T6</f>
+        <f t="shared" si="12"/>
         <v>-19135</v>
       </c>
       <c r="U22" s="33">
-        <f>U14-U6</f>
+        <f t="shared" si="12"/>
         <v>-24100</v>
       </c>
     </row>
@@ -14497,63 +14493,63 @@
         <v>0.04</v>
       </c>
       <c r="G23" s="33">
-        <f>G15-G7</f>
+        <f t="shared" ref="G23:U23" si="13">G15-G7</f>
         <v>0</v>
       </c>
       <c r="H23" s="33">
-        <f>H15-H7</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I23" s="33">
-        <f>I15-I7</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="J23" s="33">
-        <f>J15-J7</f>
+        <f t="shared" si="13"/>
         <v>-3296</v>
       </c>
       <c r="K23" s="33">
-        <f>K15-K7</f>
+        <f t="shared" si="13"/>
         <v>-3827</v>
       </c>
       <c r="L23" s="33">
-        <f>L15-L7</f>
+        <f t="shared" si="13"/>
         <v>-4820</v>
       </c>
       <c r="M23" s="33">
-        <f>M15-M7</f>
+        <f t="shared" si="13"/>
         <v>-7691</v>
       </c>
       <c r="N23" s="33">
-        <f>N15-N7</f>
+        <f t="shared" si="13"/>
         <v>-8930</v>
       </c>
       <c r="O23" s="33">
-        <f>O15-O7</f>
+        <f t="shared" si="13"/>
         <v>-11247</v>
       </c>
       <c r="P23" s="33">
-        <f>P15-P7</f>
+        <f t="shared" si="13"/>
         <v>-12086</v>
       </c>
       <c r="Q23" s="33">
-        <f>Q15-Q7</f>
+        <f t="shared" si="13"/>
         <v>-14033</v>
       </c>
       <c r="R23" s="33">
-        <f>R15-R7</f>
+        <f t="shared" si="13"/>
         <v>-17673</v>
       </c>
       <c r="S23" s="33">
-        <f>S15-S7</f>
+        <f t="shared" si="13"/>
         <v>-16481</v>
       </c>
       <c r="T23" s="33">
-        <f>T15-T7</f>
+        <f t="shared" si="13"/>
         <v>-19136</v>
       </c>
       <c r="U23" s="33">
-        <f>U15-U7</f>
+        <f t="shared" si="13"/>
         <v>-24101</v>
       </c>
     </row>
@@ -14574,63 +14570,63 @@
         <v>0.04</v>
       </c>
       <c r="G24" s="33">
-        <f>G16-G8</f>
+        <f t="shared" ref="G24:U24" si="14">G16-G8</f>
         <v>0</v>
       </c>
       <c r="H24" s="33">
-        <f>H16-H8</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I24" s="33">
-        <f>I16-I8</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J24" s="33">
-        <f>J16-J8</f>
+        <f t="shared" si="14"/>
         <v>-3586</v>
       </c>
       <c r="K24" s="33">
-        <f>K16-K8</f>
+        <f t="shared" si="14"/>
         <v>-3975</v>
       </c>
       <c r="L24" s="33">
-        <f>L16-L8</f>
+        <f t="shared" si="14"/>
         <v>-4365</v>
       </c>
       <c r="M24" s="33">
-        <f>M16-M8</f>
+        <f t="shared" si="14"/>
         <v>-8367</v>
       </c>
       <c r="N24" s="33">
-        <f>N16-N8</f>
+        <f t="shared" si="14"/>
         <v>-9275</v>
       </c>
       <c r="O24" s="33">
-        <f>O16-O8</f>
+        <f t="shared" si="14"/>
         <v>-10185</v>
       </c>
       <c r="P24" s="33">
-        <f>P16-P8</f>
+        <f t="shared" si="14"/>
         <v>-13148</v>
       </c>
       <c r="Q24" s="33">
-        <f>Q16-Q8</f>
+        <f t="shared" si="14"/>
         <v>-14576</v>
       </c>
       <c r="R24" s="33">
-        <f>R16-R8</f>
+        <f t="shared" si="14"/>
         <v>-16005</v>
       </c>
       <c r="S24" s="33">
-        <f>S16-S8</f>
+        <f t="shared" si="14"/>
         <v>-17928</v>
       </c>
       <c r="T24" s="33">
-        <f>T16-T8</f>
+        <f t="shared" si="14"/>
         <v>-19876</v>
       </c>
       <c r="U24" s="33">
-        <f>U16-U8</f>
+        <f t="shared" si="14"/>
         <v>-21825</v>
       </c>
     </row>
@@ -14651,63 +14647,63 @@
         <v>0.04</v>
       </c>
       <c r="G25" s="33">
-        <f>G17-G9</f>
+        <f t="shared" ref="G25:U25" si="15">G17-G9</f>
         <v>0</v>
       </c>
       <c r="H25" s="33">
-        <f>H17-H9</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I25" s="33">
-        <f>I17-I9</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="J25" s="33">
-        <f>J17-J9</f>
+        <f t="shared" si="15"/>
         <v>-3586</v>
       </c>
       <c r="K25" s="33">
-        <f>K17-K9</f>
+        <f t="shared" si="15"/>
         <v>-3975</v>
       </c>
       <c r="L25" s="33">
-        <f>L17-L9</f>
+        <f t="shared" si="15"/>
         <v>-4365</v>
       </c>
       <c r="M25" s="33">
-        <f>M17-M9</f>
+        <f t="shared" si="15"/>
         <v>-8366</v>
       </c>
       <c r="N25" s="33">
-        <f>N17-N9</f>
+        <f t="shared" si="15"/>
         <v>-9276</v>
       </c>
       <c r="O25" s="33">
-        <f>O17-O9</f>
+        <f t="shared" si="15"/>
         <v>-10185</v>
       </c>
       <c r="P25" s="33">
-        <f>P17-P9</f>
+        <f t="shared" si="15"/>
         <v>-13148</v>
       </c>
       <c r="Q25" s="33">
-        <f>Q17-Q9</f>
+        <f t="shared" si="15"/>
         <v>-14577</v>
       </c>
       <c r="R25" s="33">
-        <f>R17-R9</f>
+        <f t="shared" si="15"/>
         <v>-16004</v>
       </c>
       <c r="S25" s="33">
-        <f>S17-S9</f>
+        <f t="shared" si="15"/>
         <v>-17929</v>
       </c>
       <c r="T25" s="33">
-        <f>T17-T9</f>
+        <f t="shared" si="15"/>
         <v>-19877</v>
       </c>
       <c r="U25" s="33">
-        <f>U17-U9</f>
+        <f t="shared" si="15"/>
         <v>-21825</v>
       </c>
     </row>
@@ -14728,63 +14724,63 @@
         <v>0.04</v>
       </c>
       <c r="G26" s="33">
-        <f>G18-G10</f>
+        <f t="shared" ref="G26:U26" si="16">G18-G10</f>
         <v>0</v>
       </c>
       <c r="H26" s="33">
-        <f>H18-H10</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="I26" s="33">
-        <f>I18-I10</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="J26" s="33">
-        <f>J18-J10</f>
+        <f t="shared" si="16"/>
         <v>-3586</v>
       </c>
       <c r="K26" s="33">
-        <f>K18-K10</f>
+        <f t="shared" si="16"/>
         <v>-3976</v>
       </c>
       <c r="L26" s="33">
-        <f>L18-L10</f>
+        <f t="shared" si="16"/>
         <v>-4365</v>
       </c>
       <c r="M26" s="33">
-        <f>M18-M10</f>
+        <f t="shared" si="16"/>
         <v>-8367</v>
       </c>
       <c r="N26" s="33">
-        <f>N18-N10</f>
+        <f t="shared" si="16"/>
         <v>-9276</v>
       </c>
       <c r="O26" s="33">
-        <f>O18-O10</f>
+        <f t="shared" si="16"/>
         <v>-10185</v>
       </c>
       <c r="P26" s="33">
-        <f>P18-P10</f>
+        <f t="shared" si="16"/>
         <v>-13148</v>
       </c>
       <c r="Q26" s="33">
-        <f>Q18-Q10</f>
+        <f t="shared" si="16"/>
         <v>-14577</v>
       </c>
       <c r="R26" s="33">
-        <f>R18-R10</f>
+        <f t="shared" si="16"/>
         <v>-16005</v>
       </c>
       <c r="S26" s="33">
-        <f>S18-S10</f>
+        <f t="shared" si="16"/>
         <v>-17929</v>
       </c>
       <c r="T26" s="33">
-        <f>T18-T10</f>
+        <f t="shared" si="16"/>
         <v>-19876</v>
       </c>
       <c r="U26" s="33">
-        <f>U18-U10</f>
+        <f t="shared" si="16"/>
         <v>-21825</v>
       </c>
     </row>
@@ -14805,63 +14801,63 @@
         <v>0.04</v>
       </c>
       <c r="G27" s="33">
-        <f>G19-G11</f>
+        <f t="shared" ref="G27:U27" si="17">G19-G11</f>
         <v>0</v>
       </c>
       <c r="H27" s="33">
-        <f>H19-H11</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I27" s="33">
-        <f>I19-I11</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="J27" s="33">
-        <f>J19-J11</f>
+        <f t="shared" si="17"/>
         <v>-3585</v>
       </c>
       <c r="K27" s="33">
-        <f>K19-K11</f>
+        <f t="shared" si="17"/>
         <v>-3975</v>
       </c>
       <c r="L27" s="33">
-        <f>L19-L11</f>
+        <f t="shared" si="17"/>
         <v>-4365</v>
       </c>
       <c r="M27" s="33">
-        <f>M19-M11</f>
+        <f t="shared" si="17"/>
         <v>-8366</v>
       </c>
       <c r="N27" s="33">
-        <f>N19-N11</f>
+        <f t="shared" si="17"/>
         <v>-9276</v>
       </c>
       <c r="O27" s="33">
-        <f>O19-O11</f>
+        <f t="shared" si="17"/>
         <v>-10184</v>
       </c>
       <c r="P27" s="33">
-        <f>P19-P11</f>
+        <f t="shared" si="17"/>
         <v>-13148</v>
       </c>
       <c r="Q27" s="33">
-        <f>Q19-Q11</f>
+        <f t="shared" si="17"/>
         <v>-14577</v>
       </c>
       <c r="R27" s="33">
-        <f>R19-R11</f>
+        <f t="shared" si="17"/>
         <v>-16005</v>
       </c>
       <c r="S27" s="33">
-        <f>S19-S11</f>
+        <f t="shared" si="17"/>
         <v>-17928</v>
       </c>
       <c r="T27" s="33">
-        <f>T19-T11</f>
+        <f t="shared" si="17"/>
         <v>-19877</v>
       </c>
       <c r="U27" s="33">
-        <f>U19-U11</f>
+        <f t="shared" si="17"/>
         <v>-21825</v>
       </c>
     </row>
@@ -14870,6 +14866,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="AN1:AS1"/>
+    <mergeCell ref="AT1:AY1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G3:U3"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="S1:U1"/>
     <mergeCell ref="X3:AA3"/>
     <mergeCell ref="AZ1:BE1"/>
     <mergeCell ref="X2:AA2"/>
@@ -14886,16 +14892,6 @@
     <mergeCell ref="X1:AA1"/>
     <mergeCell ref="AB1:AG1"/>
     <mergeCell ref="AH1:AM1"/>
-    <mergeCell ref="AN1:AS1"/>
-    <mergeCell ref="AT1:AY1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G3:U3"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="S1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -14911,7 +14907,7 @@
   <dimension ref="B1:AJ40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AI5" sqref="AI5"/>
+      <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14934,51 +14930,51 @@
   <sheetData>
     <row r="1" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="77" t="s">
+      <c r="C2" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="79" t="s">
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77" t="s">
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77" t="s">
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="77"/>
-      <c r="P2" s="77"/>
-      <c r="Q2" s="77" t="s">
+      <c r="O2" s="72"/>
+      <c r="P2" s="72"/>
+      <c r="Q2" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="77"/>
-      <c r="S2" s="77"/>
-      <c r="T2" s="77" t="s">
+      <c r="R2" s="72"/>
+      <c r="S2" s="72"/>
+      <c r="T2" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="U2" s="77"/>
-      <c r="V2" s="78"/>
+      <c r="U2" s="72"/>
+      <c r="V2" s="83"/>
     </row>
     <row r="3" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="72"/>
+      <c r="B3" s="78"/>
       <c r="C3" s="67" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="67"/>
       <c r="E3" s="67"/>
       <c r="F3" s="67"/>
-      <c r="G3" s="80"/>
+      <c r="G3" s="85"/>
       <c r="H3" s="1">
         <v>4.5999999999999996</v>
       </c>
@@ -15026,7 +15022,7 @@
       </c>
     </row>
     <row r="4" spans="2:36" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="73"/>
+      <c r="B4" s="79"/>
       <c r="C4" s="10" t="s">
         <v>7</v>
       </c>
@@ -15042,7 +15038,7 @@
       <c r="G4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="70" t="s">
+      <c r="H4" s="68" t="s">
         <v>91</v>
       </c>
       <c r="I4" s="67"/>
@@ -15058,7 +15054,7 @@
       <c r="S4" s="67"/>
       <c r="T4" s="67"/>
       <c r="U4" s="67"/>
-      <c r="V4" s="80"/>
+      <c r="V4" s="85"/>
       <c r="X4" s="49"/>
       <c r="Y4" s="49"/>
       <c r="Z4" s="49"/>
@@ -15137,11 +15133,11 @@
         <v>13690</v>
       </c>
       <c r="X5" s="57">
-        <f t="shared" ref="X5:AI12" si="0">(K5-K13)/K5*100</f>
+        <f>(K5-K13)/K5*100</f>
         <v>27.778245850535004</v>
       </c>
       <c r="Y5" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="X5:AI12" si="0">(L5-L13)/L5*100</f>
         <v>33.661711672090775</v>
       </c>
       <c r="Z5" s="58">
@@ -15184,7 +15180,7 @@
         <f>(V5-V13)/V5*100</f>
         <v>176.0482103725347</v>
       </c>
-      <c r="AJ5" s="82" t="s">
+      <c r="AJ5" s="74" t="s">
         <v>95</v>
       </c>
     </row>
@@ -15300,7 +15296,7 @@
         <f t="shared" si="0"/>
         <v>164.40412033562998</v>
       </c>
-      <c r="AJ6" s="83"/>
+      <c r="AJ6" s="75"/>
     </row>
     <row r="7" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="12">
@@ -15414,7 +15410,7 @@
         <f t="shared" si="0"/>
         <v>157.60528380852733</v>
       </c>
-      <c r="AJ7" s="83"/>
+      <c r="AJ7" s="75"/>
     </row>
     <row r="8" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="12">
@@ -15528,7 +15524,7 @@
         <f t="shared" si="0"/>
         <v>155.26349697203969</v>
       </c>
-      <c r="AJ8" s="83"/>
+      <c r="AJ8" s="75"/>
     </row>
     <row r="9" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="12">
@@ -15642,7 +15638,7 @@
         <f t="shared" si="0"/>
         <v>110.82618189204285</v>
       </c>
-      <c r="AJ9" s="83"/>
+      <c r="AJ9" s="75"/>
     </row>
     <row r="10" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="12">
@@ -15756,7 +15752,7 @@
         <f t="shared" si="0"/>
         <v>103.22077185017027</v>
       </c>
-      <c r="AJ10" s="83"/>
+      <c r="AJ10" s="75"/>
     </row>
     <row r="11" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="12">
@@ -15870,7 +15866,7 @@
         <f t="shared" si="0"/>
         <v>99.839890210429999</v>
       </c>
-      <c r="AJ11" s="83"/>
+      <c r="AJ11" s="75"/>
     </row>
     <row r="12" spans="2:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="12">
@@ -15984,7 +15980,7 @@
         <f t="shared" si="0"/>
         <v>97.861082462669842</v>
       </c>
-      <c r="AJ12" s="84"/>
+      <c r="AJ12" s="76"/>
     </row>
     <row r="13" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="12">
@@ -16062,7 +16058,7 @@
       <c r="AG13" s="48"/>
       <c r="AH13" s="48"/>
       <c r="AI13" s="48"/>
-      <c r="AJ13" s="81"/>
+      <c r="AJ13" s="73"/>
     </row>
     <row r="14" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="12">
@@ -16140,7 +16136,7 @@
       <c r="AG14" s="48"/>
       <c r="AH14" s="48"/>
       <c r="AI14" s="48"/>
-      <c r="AJ14" s="81"/>
+      <c r="AJ14" s="73"/>
     </row>
     <row r="15" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="12">
@@ -16218,7 +16214,7 @@
       <c r="AG15" s="48"/>
       <c r="AH15" s="48"/>
       <c r="AI15" s="48"/>
-      <c r="AJ15" s="81"/>
+      <c r="AJ15" s="73"/>
     </row>
     <row r="16" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="12">
@@ -16296,7 +16292,7 @@
       <c r="AG16" s="48"/>
       <c r="AH16" s="48"/>
       <c r="AI16" s="48"/>
-      <c r="AJ16" s="81"/>
+      <c r="AJ16" s="73"/>
     </row>
     <row r="17" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="12">
@@ -16374,7 +16370,7 @@
       <c r="AG17" s="48"/>
       <c r="AH17" s="48"/>
       <c r="AI17" s="48"/>
-      <c r="AJ17" s="81"/>
+      <c r="AJ17" s="73"/>
     </row>
     <row r="18" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="12">
@@ -16452,7 +16448,7 @@
       <c r="AG18" s="48"/>
       <c r="AH18" s="48"/>
       <c r="AI18" s="48"/>
-      <c r="AJ18" s="81"/>
+      <c r="AJ18" s="73"/>
     </row>
     <row r="19" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="12">
@@ -16530,7 +16526,7 @@
       <c r="AG19" s="48"/>
       <c r="AH19" s="48"/>
       <c r="AI19" s="48"/>
-      <c r="AJ19" s="81"/>
+      <c r="AJ19" s="73"/>
     </row>
     <row r="20" spans="2:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="13">
@@ -16608,7 +16604,7 @@
       <c r="AG20" s="48"/>
       <c r="AH20" s="48"/>
       <c r="AI20" s="48"/>
-      <c r="AJ20" s="81"/>
+      <c r="AJ20" s="73"/>
     </row>
     <row r="21" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="X21" s="48"/>
@@ -16625,41 +16621,41 @@
       <c r="AI21" s="48"/>
     </row>
     <row r="22" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="74" t="s">
+      <c r="B22" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="77" t="s">
+      <c r="C22" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="77"/>
-      <c r="E22" s="77"/>
-      <c r="F22" s="77"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="79" t="s">
+      <c r="D22" s="72"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="83"/>
+      <c r="H22" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="I22" s="77"/>
-      <c r="J22" s="77"/>
-      <c r="K22" s="77" t="s">
+      <c r="I22" s="72"/>
+      <c r="J22" s="72"/>
+      <c r="K22" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="L22" s="77"/>
-      <c r="M22" s="77"/>
-      <c r="N22" s="77" t="s">
+      <c r="L22" s="72"/>
+      <c r="M22" s="72"/>
+      <c r="N22" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="O22" s="77"/>
-      <c r="P22" s="77"/>
-      <c r="Q22" s="77" t="s">
+      <c r="O22" s="72"/>
+      <c r="P22" s="72"/>
+      <c r="Q22" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="R22" s="77"/>
-      <c r="S22" s="77"/>
-      <c r="T22" s="77" t="s">
+      <c r="R22" s="72"/>
+      <c r="S22" s="72"/>
+      <c r="T22" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="U22" s="77"/>
-      <c r="V22" s="78"/>
+      <c r="U22" s="72"/>
+      <c r="V22" s="83"/>
       <c r="X22" s="48"/>
       <c r="Y22" s="48"/>
       <c r="Z22" s="48"/>
@@ -16674,14 +16670,14 @@
       <c r="AI22" s="48"/>
     </row>
     <row r="23" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="75"/>
+      <c r="B23" s="81"/>
       <c r="C23" s="67" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="67"/>
       <c r="E23" s="67"/>
       <c r="F23" s="67"/>
-      <c r="G23" s="80"/>
+      <c r="G23" s="85"/>
       <c r="H23" s="1">
         <v>4.5999999999999996</v>
       </c>
@@ -16741,7 +16737,7 @@
       <c r="AI23" s="48"/>
     </row>
     <row r="24" spans="2:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="76"/>
+      <c r="B24" s="82"/>
       <c r="C24" s="10" t="s">
         <v>7</v>
       </c>
@@ -16757,7 +16753,7 @@
       <c r="G24" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="70" t="s">
+      <c r="H24" s="68" t="s">
         <v>92</v>
       </c>
       <c r="I24" s="67"/>
@@ -16773,7 +16769,7 @@
       <c r="S24" s="67"/>
       <c r="T24" s="67"/>
       <c r="U24" s="67"/>
-      <c r="V24" s="80"/>
+      <c r="V24" s="85"/>
       <c r="X24" s="49"/>
       <c r="Y24" s="49"/>
       <c r="Z24" s="49"/>
@@ -16899,7 +16895,7 @@
         <f t="shared" si="1"/>
         <v>160.54893078409168</v>
       </c>
-      <c r="AJ25" s="82" t="s">
+      <c r="AJ25" s="74" t="s">
         <v>95</v>
       </c>
     </row>
@@ -16976,7 +16972,7 @@
         <v>29.703508227258613</v>
       </c>
       <c r="Z26" s="61">
-        <f t="shared" ref="Z26:Z32" si="4">(M26-M34)/M26*100</f>
+        <f t="shared" ref="Z26:Z31" si="4">(M26-M34)/M26*100</f>
         <v>40.334728033472807</v>
       </c>
       <c r="AA26" s="61">
@@ -17015,7 +17011,7 @@
         <f t="shared" ref="AI26:AI32" si="13">(V26-V34)/V26*100</f>
         <v>150.81033727551468</v>
       </c>
-      <c r="AJ26" s="83"/>
+      <c r="AJ26" s="75"/>
     </row>
     <row r="27" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="12">
@@ -17129,7 +17125,7 @@
         <f t="shared" si="13"/>
         <v>145.06711611388673</v>
       </c>
-      <c r="AJ27" s="83"/>
+      <c r="AJ27" s="75"/>
     </row>
     <row r="28" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="12">
@@ -17243,7 +17239,7 @@
         <f t="shared" si="13"/>
         <v>143.08359059605795</v>
       </c>
-      <c r="AJ28" s="83"/>
+      <c r="AJ28" s="75"/>
     </row>
     <row r="29" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="12">
@@ -17357,7 +17353,7 @@
         <f t="shared" si="13"/>
         <v>103.85933187398876</v>
       </c>
-      <c r="AJ29" s="83"/>
+      <c r="AJ29" s="75"/>
     </row>
     <row r="30" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="12">
@@ -17471,7 +17467,7 @@
         <f t="shared" si="13"/>
         <v>97.146799608296988</v>
       </c>
-      <c r="AJ30" s="83"/>
+      <c r="AJ30" s="75"/>
     </row>
     <row r="31" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="12">
@@ -17585,7 +17581,7 @@
         <f t="shared" si="13"/>
         <v>94.150381778180403</v>
       </c>
-      <c r="AJ31" s="83"/>
+      <c r="AJ31" s="75"/>
     </row>
     <row r="32" spans="2:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="12">
@@ -17699,7 +17695,7 @@
         <f t="shared" si="13"/>
         <v>92.388773652796004</v>
       </c>
-      <c r="AJ32" s="84"/>
+      <c r="AJ32" s="76"/>
     </row>
     <row r="33" spans="2:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="12">
@@ -18327,11 +18323,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="AJ13:AJ20"/>
-    <mergeCell ref="AJ5:AJ12"/>
-    <mergeCell ref="AJ25:AJ32"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="C2:G2"/>
@@ -18348,6 +18339,11 @@
     <mergeCell ref="Q22:S22"/>
     <mergeCell ref="T22:V22"/>
     <mergeCell ref="T2:V2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="AJ13:AJ20"/>
+    <mergeCell ref="AJ5:AJ12"/>
+    <mergeCell ref="AJ25:AJ32"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:V20">
     <cfRule type="colorScale" priority="2">
@@ -18416,13 +18412,13 @@
       <c r="G2" s="20"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
       <c r="G3" s="20"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -18786,12 +18782,12 @@
       <c r="G25" s="20"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="86" t="s">
+      <c r="B26" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="86"/>
-      <c r="D26" s="86"/>
-      <c r="E26" s="86"/>
+      <c r="C26" s="87"/>
+      <c r="D26" s="87"/>
+      <c r="E26" s="87"/>
       <c r="F26" s="31"/>
       <c r="G26" s="20"/>
     </row>

</xml_diff>